<commit_message>
Updated tourism data. Includes sum within islands for BES, KNA and TTO
</commit_message>
<xml_diff>
--- a/raw_data/tourism/cto_2015_tourism.xlsx
+++ b/raw_data/tourism/cto_2015_tourism.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmlawson/github/kuni_fads/raw_data/tourism/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED9CE75-064D-2D42-9457-D35B3B8DD05A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855A09A0-81B4-6E49-97DA-0D043CADBD38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="460" windowWidth="25000" windowHeight="15000" xr2:uid="{F6B79E57-BD6F-1745-BBF6-B82E6441DBA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
   <si>
     <t>name</t>
   </si>
@@ -54,15 +54,6 @@
     <t>Bonaire, Sint Eustatius and Saba</t>
   </si>
   <si>
-    <t>Bonaire</t>
-  </si>
-  <si>
-    <t>Sint Eustatius</t>
-  </si>
-  <si>
-    <t>Saba</t>
-  </si>
-  <si>
     <t>Cayman Islands</t>
   </si>
   <si>
@@ -105,12 +96,6 @@
     <t>Saint Kitts and Nevis</t>
   </si>
   <si>
-    <t>Saint Kitts</t>
-  </si>
-  <si>
-    <t>Nevis</t>
-  </si>
-  <si>
     <t>Saint Lucia</t>
   </si>
   <si>
@@ -126,12 +111,6 @@
     <t>Trinidad and Tobago</t>
   </si>
   <si>
-    <t>Trinidad</t>
-  </si>
-  <si>
-    <t>Tobago</t>
-  </si>
-  <si>
     <t>Turks and Caicos Islands</t>
   </si>
   <si>
@@ -235,9 +214,6 @@
   </si>
   <si>
     <t>VIR</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -628,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4397B5D7-63E7-D345-865B-A840F50A8124}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,19 +620,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -667,7 +643,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <v>660</v>
@@ -684,7 +660,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D3">
         <v>27</v>
@@ -701,7 +677,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>533</v>
@@ -718,7 +694,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D5">
         <v>44</v>
@@ -735,7 +711,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D6">
         <v>52</v>
@@ -752,64 +728,64 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>535</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>68</v>
+      <c r="E7" s="6">
+        <v>168100</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D8">
-        <v>535</v>
+        <v>136</v>
       </c>
       <c r="E8" s="6">
-        <v>133000</v>
+        <v>382816</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D9">
-        <v>535</v>
+        <v>192</v>
       </c>
       <c r="E9" s="6">
-        <v>14600</v>
+        <v>3001958</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>6</v>
+      <c r="A10" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D10">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="E10" s="6">
-        <v>20500</v>
+        <v>450953</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -820,13 +796,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D11">
-        <v>136</v>
+        <v>212</v>
       </c>
       <c r="E11" s="6">
-        <v>382816</v>
+        <v>81472</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -837,30 +813,30 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D12">
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="E12" s="6">
-        <v>3001958</v>
+        <v>5141377</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D13">
-        <v>531</v>
+        <v>308</v>
       </c>
       <c r="E13" s="6">
-        <v>450953</v>
+        <v>133521</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -871,13 +847,13 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D14">
-        <v>212</v>
+        <v>312</v>
       </c>
       <c r="E14" s="6">
-        <v>81472</v>
+        <v>487000</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -888,13 +864,13 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D15">
-        <v>214</v>
+        <v>332</v>
       </c>
       <c r="E15" s="6">
-        <v>5141377</v>
+        <v>465174</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -905,13 +881,13 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D16">
-        <v>308</v>
+        <v>388</v>
       </c>
       <c r="E16" s="6">
-        <v>133521</v>
+        <v>2080181</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -922,13 +898,13 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D17">
-        <v>312</v>
+        <v>474</v>
       </c>
       <c r="E17" s="6">
-        <v>487000</v>
+        <v>489561</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -939,13 +915,13 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D18">
-        <v>332</v>
+        <v>500</v>
       </c>
       <c r="E18" s="6">
-        <v>465174</v>
+        <v>8804</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -956,30 +932,30 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D19">
-        <v>388</v>
+        <v>630</v>
       </c>
       <c r="E19" s="6">
-        <v>2080181</v>
+        <v>1688472</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D20">
-        <v>474</v>
+        <v>652</v>
       </c>
       <c r="E20" s="6">
-        <v>489561</v>
+        <v>281272</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -990,13 +966,13 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D21">
-        <v>500</v>
+        <v>659</v>
       </c>
       <c r="E21" s="6">
-        <v>8804</v>
+        <v>104730</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1007,30 +983,30 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D22">
-        <v>630</v>
+        <v>662</v>
       </c>
       <c r="E22" s="6">
-        <v>1688472</v>
+        <v>338158</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D23">
-        <v>652</v>
+        <v>663</v>
       </c>
       <c r="E23" s="6">
-        <v>281272</v>
+        <v>201219</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1041,47 +1017,47 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D24">
-        <v>659</v>
+        <v>670</v>
       </c>
       <c r="E24" s="6">
-        <v>104730</v>
+        <v>70713</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="A25" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D25">
-        <v>659</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>68</v>
+        <v>534</v>
+      </c>
+      <c r="E25" s="6">
+        <v>499920</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="B26" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D26">
-        <v>659</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>68</v>
+        <v>780</v>
+      </c>
+      <c r="E26" s="6">
+        <v>412537</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1092,165 +1068,46 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D27">
-        <v>662</v>
+        <v>796</v>
       </c>
       <c r="E27" s="6">
-        <v>338158</v>
+        <v>368164</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D28">
-        <v>663</v>
+        <v>92</v>
       </c>
       <c r="E28" s="6">
-        <v>201219</v>
+        <v>386049</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D29">
-        <v>670</v>
+        <v>850</v>
       </c>
       <c r="E29" s="6">
-        <v>70713</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30">
-        <v>534</v>
-      </c>
-      <c r="E30" s="6">
-        <v>499920</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31">
-        <v>780</v>
-      </c>
-      <c r="E31" s="6">
-        <v>412537</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32">
-        <v>780</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33">
-        <v>780</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34">
-        <v>796</v>
-      </c>
-      <c r="E34" s="6">
-        <v>368164</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" t="s">
-        <v>66</v>
-      </c>
-      <c r="D35">
-        <v>92</v>
-      </c>
-      <c r="E35" s="6">
-        <v>386049</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36">
-        <v>850</v>
-      </c>
-      <c r="E36" s="6">
         <v>730367</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating data and plots
</commit_message>
<xml_diff>
--- a/raw_data/tourism/cto_2015_tourism.xlsx
+++ b/raw_data/tourism/cto_2015_tourism.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmlawson/github/kuni_fads/raw_data/tourism/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretwilson/github/kuni_fads/raw_data/tourism/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855A09A0-81B4-6E49-97DA-0D043CADBD38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0CB13D-8332-C144-AFE7-A101ECF24A4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="25000" windowHeight="15000" xr2:uid="{F6B79E57-BD6F-1745-BBF6-B82E6441DBA3}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="25000" windowHeight="14180" xr2:uid="{F6B79E57-BD6F-1745-BBF6-B82E6441DBA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
   <si>
     <t>name</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>VIR</t>
+  </si>
+  <si>
+    <t>BMU</t>
+  </si>
+  <si>
+    <t>Bermuda</t>
   </si>
 </sst>
 </file>
@@ -604,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4397B5D7-63E7-D345-865B-A840F50A8124}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1111,6 +1117,23 @@
         <v>730367</v>
       </c>
     </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30">
+        <v>3166</v>
+      </c>
+      <c r="E30" s="6">
+        <v>142924</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
leaving slots for B/E/S in tourism data
</commit_message>
<xml_diff>
--- a/raw_data/tourism/cto_2015_tourism.xlsx
+++ b/raw_data/tourism/cto_2015_tourism.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretwilson/github/kuni_fads/raw_data/tourism/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0CB13D-8332-C144-AFE7-A101ECF24A4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1225D224-B73F-A14E-B092-5BBC8903A519}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="460" windowWidth="25000" windowHeight="14180" xr2:uid="{F6B79E57-BD6F-1745-BBF6-B82E6441DBA3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
   <si>
     <t>name</t>
   </si>
@@ -147,9 +147,6 @@
     <t>BRB</t>
   </si>
   <si>
-    <t>BES</t>
-  </si>
-  <si>
     <t>CYM</t>
   </si>
   <si>
@@ -220,6 +217,24 @@
   </si>
   <si>
     <t>Bermuda</t>
+  </si>
+  <si>
+    <t>Sint Eustatius</t>
+  </si>
+  <si>
+    <t>Saba</t>
+  </si>
+  <si>
+    <t>Bonaire</t>
+  </si>
+  <si>
+    <t>BESB</t>
+  </si>
+  <si>
+    <t>BESE</t>
+  </si>
+  <si>
+    <t>BESS</t>
   </si>
 </sst>
 </file>
@@ -610,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4397B5D7-63E7-D345-865B-A840F50A8124}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -731,406 +746,431 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="D7">
         <v>535</v>
       </c>
-      <c r="E7" s="6">
-        <v>168100</v>
-      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="D8">
-        <v>136</v>
-      </c>
-      <c r="E8" s="6">
-        <v>382816</v>
+        <v>535</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D9">
-        <v>192</v>
-      </c>
-      <c r="E9" s="6">
-        <v>3001958</v>
+        <v>535</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D10">
-        <v>531</v>
+        <v>136</v>
       </c>
       <c r="E10" s="6">
-        <v>450953</v>
+        <v>382816</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D11">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="E11" s="6">
-        <v>81472</v>
+        <v>3001958</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>11</v>
+      <c r="A12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D12">
-        <v>214</v>
+        <v>531</v>
       </c>
       <c r="E12" s="6">
-        <v>5141377</v>
+        <v>450953</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D13">
-        <v>308</v>
+        <v>212</v>
       </c>
       <c r="E13" s="6">
-        <v>133521</v>
+        <v>81472</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D14">
-        <v>312</v>
+        <v>214</v>
       </c>
       <c r="E14" s="6">
-        <v>487000</v>
+        <v>5141377</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D15">
-        <v>332</v>
+        <v>308</v>
       </c>
       <c r="E15" s="6">
-        <v>465174</v>
+        <v>133521</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D16">
-        <v>388</v>
+        <v>312</v>
       </c>
       <c r="E16" s="6">
-        <v>2080181</v>
+        <v>487000</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D17">
-        <v>474</v>
+        <v>332</v>
       </c>
       <c r="E17" s="6">
-        <v>489561</v>
+        <v>465174</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D18">
-        <v>500</v>
+        <v>388</v>
       </c>
       <c r="E18" s="6">
-        <v>8804</v>
+        <v>2080181</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D19">
-        <v>630</v>
+        <v>474</v>
       </c>
       <c r="E19" s="6">
-        <v>1688472</v>
+        <v>489561</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>19</v>
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D20">
-        <v>652</v>
+        <v>500</v>
       </c>
       <c r="E20" s="6">
-        <v>281272</v>
+        <v>8804</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21">
+        <v>630</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1688472</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22">
+        <v>652</v>
+      </c>
+      <c r="E22" s="6">
+        <v>281272</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21">
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23">
         <v>659</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E23" s="6">
         <v>104730</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22">
-        <v>662</v>
-      </c>
-      <c r="E22" s="6">
-        <v>338158</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23">
-        <v>663</v>
-      </c>
-      <c r="E23" s="6">
-        <v>201219</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D24">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="E24" s="6">
-        <v>70713</v>
+        <v>338158</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D25">
-        <v>534</v>
+        <v>663</v>
       </c>
       <c r="E25" s="6">
-        <v>499920</v>
+        <v>201219</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D26">
-        <v>780</v>
+        <v>670</v>
       </c>
       <c r="E26" s="6">
-        <v>412537</v>
+        <v>70713</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>26</v>
+      <c r="A27" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D27">
-        <v>796</v>
+        <v>534</v>
       </c>
       <c r="E27" s="6">
-        <v>368164</v>
+        <v>499920</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D28">
-        <v>92</v>
+        <v>780</v>
       </c>
       <c r="E28" s="6">
-        <v>386049</v>
+        <v>412537</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>28</v>
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D29">
-        <v>850</v>
+        <v>796</v>
       </c>
       <c r="E29" s="6">
-        <v>730367</v>
+        <v>368164</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30">
+        <v>92</v>
+      </c>
+      <c r="E30" s="6">
+        <v>386049</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31">
+        <v>850</v>
+      </c>
+      <c r="E31" s="6">
+        <v>730367</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>61</v>
       </c>
-      <c r="D30">
+      <c r="B32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32">
         <v>3166</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E32" s="6">
         <v>142924</v>
       </c>
     </row>

</xml_diff>